<commit_message>
add 我的，after logon model
</commit_message>
<xml_diff>
--- a/flowernut_plan.xlsx
+++ b/flowernut_plan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
   <si>
     <t>人员</t>
   </si>
@@ -97,21 +97,6 @@
     <t>显示用户信息</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>招聘技师？ 是像享在家一样，把技师招聘进来，还是让技师自己注册，我们审批？像拼车平台，车主和乘客都是自己注册？</t>
-    </r>
-  </si>
-  <si>
     <t>about us</t>
   </si>
   <si>
@@ -140,9 +125,6 @@
   </si>
   <si>
     <t>留个邮箱</t>
-  </si>
-  <si>
-    <t>首页下面的菜单： 首页，我的，更多</t>
   </si>
   <si>
     <t>更多</t>
@@ -259,6 +241,54 @@
         <charset val="134"/>
       </rPr>
       <t>核心业务流程：提供一个平台，让催乳技师和普通用户能够方便的联系。</t>
+    </r>
+  </si>
+  <si>
+    <t>我的</t>
+  </si>
+  <si>
+    <t>个人资料</t>
+  </si>
+  <si>
+    <t>优惠卷</t>
+  </si>
+  <si>
+    <t>常用地址</t>
+  </si>
+  <si>
+    <t>修改密码</t>
+  </si>
+  <si>
+    <t>订单</t>
+  </si>
+  <si>
+    <t>全部</t>
+  </si>
+  <si>
+    <t>待付款</t>
+  </si>
+  <si>
+    <t>进行中</t>
+  </si>
+  <si>
+    <t>已完成</t>
+  </si>
+  <si>
+    <t>首页下面的菜单： 首页，我的，更多； 把 ‘订单’ 放到 ‘我的’ 里面</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>招聘技师？ 是像享在家一样，把技师招聘进来，还是让技师自己注册，我们审批？像拼车平台，车主和乘客都是自己注册？这里要决定一个技师登陆后的页面以及可以做的流程</t>
     </r>
   </si>
 </sst>
@@ -404,7 +434,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -448,6 +478,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -820,7 +853,7 @@
         <v>8</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>9</v>
@@ -835,7 +868,7 @@
         <v>12</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1014,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:G32"/>
+  <dimension ref="A4:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1031,7 +1064,7 @@
   <sheetData>
     <row r="4" spans="1:7">
       <c r="G4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1043,33 +1076,33 @@
         <v>17</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1079,18 +1112,18 @@
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="G7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="17" t="s">
@@ -1107,7 +1140,7 @@
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1130,165 +1163,159 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>31</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="13"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1"/>
-      <c r="B13" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>27</v>
-      </c>
+      <c r="B13" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="13"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1"/>
-      <c r="B14" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>35</v>
-      </c>
+      <c r="B14" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="1"/>
+      <c r="B15" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="13"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>45</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="13"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="1"/>
-      <c r="B17" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>47</v>
-      </c>
+      <c r="A17" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="13"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="B18" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="13"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>44</v>
-      </c>
+      <c r="A19" s="1"/>
+      <c r="B19" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="13"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1"/>
-      <c r="B20" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>48</v>
-      </c>
+      <c r="B20" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="13"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1"/>
-      <c r="B21" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>43</v>
-      </c>
+      <c r="B21" s="15"/>
+      <c r="C21" s="13"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="A22" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>30</v>
+      </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="1"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>26</v>
+      </c>
       <c r="D23" s="1"/>
-      <c r="E23" s="13" t="s">
-        <v>51</v>
-      </c>
+      <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+      <c r="B24" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>34</v>
+      </c>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>57</v>
-      </c>
+      <c r="A25" s="1"/>
+      <c r="B25" s="14"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="A26" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>43</v>
+      </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="A27" s="1"/>
+      <c r="B27" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>45</v>
+      </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
     </row>
@@ -1300,38 +1327,134 @@
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="A29" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+      <c r="B30" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>46</v>
+      </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" s="1"/>
+      <c r="A31" s="1"/>
+      <c r="B31" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>41</v>
+      </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1"/>
-      <c r="B32" s="13" t="s">
-        <v>62</v>
-      </c>
+      <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="1"/>
+      <c r="B42" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>